<commit_message>
Updated data with Gaussian line
</commit_message>
<xml_diff>
--- a/Report/Data.xlsx
+++ b/Report/Data.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hamza Zamani\Google Drive (hwzamani@g.ucla.edu)\UCLA\Classes\Winter2019_ECE214A\Project\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76072217-B222-47B5-8FD5-3352C7BDAA78}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15375" windowHeight="5873" xr2:uid="{D422B5F2-BC56-4908-8A15-AEBACB4A8502}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15375" windowHeight="5880"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="26">
   <si>
     <t>Train</t>
   </si>
@@ -97,12 +91,18 @@
   </si>
   <si>
     <t>Avg MFCC (12 coeff) + Avg Delta + 500 knn</t>
+  </si>
+  <si>
+    <t>Avg MFCC (13 coeff) + Delta + GMM [1] + 65 knn</t>
+  </si>
+  <si>
+    <t>Avg MFCC (13 coeff) + Delta + Delta Delta + GMM (1) + 100 knn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -132,10 +132,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -443,31 +446,31 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C17FEF67-01CB-4BD3-814E-AE2036E8F85F}">
-  <dimension ref="A1:N35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.9296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.9296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.86328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.9296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.86328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -487,7 +490,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
@@ -504,7 +507,7 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -542,7 +545,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -580,7 +583,7 @@
         <v>47.467199999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -618,7 +621,7 @@
         <v>48.148099999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -638,7 +641,7 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
@@ -655,7 +658,7 @@
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -693,7 +696,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -731,7 +734,7 @@
         <v>48.8889</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -769,7 +772,7 @@
         <v>46.341500000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -789,7 +792,7 @@
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B14" s="1" t="s">
         <v>6</v>
       </c>
@@ -806,7 +809,7 @@
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -844,7 +847,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -882,7 +885,7 @@
         <v>49.468400000000003</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -920,7 +923,7 @@
         <v>47.407400000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
@@ -940,7 +943,7 @@
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B20" s="1" t="s">
         <v>6</v>
       </c>
@@ -957,7 +960,7 @@
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -995,7 +998,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -1033,7 +1036,7 @@
         <v>49.629600000000003</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -1071,7 +1074,7 @@
         <v>47.407400000000003</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>19</v>
       </c>
@@ -1091,7 +1094,7 @@
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B26" s="1" t="s">
         <v>6</v>
       </c>
@@ -1108,7 +1111,7 @@
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -1146,7 +1149,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -1184,7 +1187,7 @@
         <v>41.481499999999997</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -1222,7 +1225,7 @@
         <v>45.185200000000002</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>22</v>
       </c>
@@ -1236,7 +1239,7 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:14" ht="14.25" x14ac:dyDescent="0.45">
       <c r="B32" s="1" t="s">
         <v>6</v>
       </c>
@@ -1248,7 +1251,7 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -1274,7 +1277,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>4</v>
       </c>
@@ -1300,7 +1303,7 @@
         <v>41.481499999999997</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:9" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -1326,18 +1329,124 @@
         <v>45.185200000000002</v>
       </c>
     </row>
+    <row r="37" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="F37" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B38" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="G38" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>2</v>
+      </c>
+      <c r="D39" t="s">
+        <v>3</v>
+      </c>
+      <c r="F39" t="s">
+        <v>0</v>
+      </c>
+      <c r="G39" t="s">
+        <v>1</v>
+      </c>
+      <c r="H39" t="s">
+        <v>2</v>
+      </c>
+      <c r="I39" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40">
+        <v>22.222000000000001</v>
+      </c>
+      <c r="C40">
+        <v>29.649000000000001</v>
+      </c>
+      <c r="D40">
+        <v>37.777000000000001</v>
+      </c>
+      <c r="F40" t="s">
+        <v>4</v>
+      </c>
+      <c r="G40">
+        <v>15.55</v>
+      </c>
+      <c r="H40">
+        <v>29.41</v>
+      </c>
+      <c r="I40">
+        <v>35.549999999999997</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41">
+        <v>33.332999999999998</v>
+      </c>
+      <c r="C41">
+        <v>25</v>
+      </c>
+      <c r="D41">
+        <v>46.654000000000003</v>
+      </c>
+      <c r="F41" t="s">
+        <v>5</v>
+      </c>
+      <c r="G41">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="H41">
+        <v>23.33</v>
+      </c>
+      <c r="I41">
+        <v>47.65</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="K19:N19"/>
-    <mergeCell ref="L20:N20"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="F7:I7"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="A19:D19"/>
+  <mergeCells count="38">
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="G38:I38"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="G32:I32"/>
     <mergeCell ref="K25:N25"/>
     <mergeCell ref="L26:N26"/>
     <mergeCell ref="A1:D1"/>
@@ -1354,14 +1463,16 @@
     <mergeCell ref="G14:I14"/>
     <mergeCell ref="K13:N13"/>
     <mergeCell ref="L14:N14"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="K19:N19"/>
+    <mergeCell ref="L20:N20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>